<commit_message>
Storing User data in a bash file and improving the overall speed of querying
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+  <si>
+    <t>#</t>
+  </si>
   <si>
     <t>ID</t>
   </si>
@@ -95,67 +98,70 @@
     <t>Jeddah</t>
   </si>
   <si>
-    <t>zahrani</t>
-  </si>
-  <si>
-    <t>zahr@sas.sa</t>
-  </si>
-  <si>
-    <t>0569988522</t>
-  </si>
-  <si>
-    <t>Accountant</t>
-  </si>
-  <si>
-    <t>Consultant</t>
+    <t>mansour</t>
+  </si>
+  <si>
+    <t>fash</t>
+  </si>
+  <si>
+    <t>mansour@sas.co</t>
+  </si>
+  <si>
+    <t>0505464613</t>
+  </si>
+  <si>
+    <t>Receptionist</t>
+  </si>
+  <si>
+    <t>Public Relations</t>
+  </si>
+  <si>
+    <t>Abha</t>
+  </si>
+  <si>
+    <t>mohammed</t>
+  </si>
+  <si>
+    <t>idreas</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>mho@sas.sa</t>
+  </si>
+  <si>
+    <t>0560798998</t>
+  </si>
+  <si>
+    <t>Network Engineer</t>
   </si>
   <si>
     <t>Automation</t>
   </si>
   <si>
-    <t>mansour</t>
-  </si>
-  <si>
-    <t>fash</t>
-  </si>
-  <si>
-    <t>mansour@sas.co</t>
-  </si>
-  <si>
-    <t>0505464613</t>
-  </si>
-  <si>
-    <t>Receptionist</t>
-  </si>
-  <si>
-    <t>Public Relations</t>
-  </si>
-  <si>
-    <t>Abha</t>
-  </si>
-  <si>
-    <t>adnan</t>
-  </si>
-  <si>
-    <t>hattab</t>
-  </si>
-  <si>
-    <t>ahattab@sas.sa</t>
-  </si>
-  <si>
-    <t>0505605505</t>
-  </si>
-  <si>
-    <t>HR Manager</t>
-  </si>
-  <si>
-    <t>manager</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
     <t>SAS</t>
+  </si>
+  <si>
+    <t>Dammam</t>
+  </si>
+  <si>
+    <t>imtiaz</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>imtiaz@sas.sa</t>
+  </si>
+  <si>
+    <t>0546467949</t>
+  </si>
+  <si>
+    <t>Business Trip</t>
+  </si>
+  <si>
+    <t>Summation</t>
   </si>
 </sst>
 </file>
@@ -200,28 +206,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="9.95703125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="10.73828125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.43359375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.22265625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="18.1484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.0546875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.86328125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.33203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="10.73046875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="27.59765625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="6.49609375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="14.66796875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="7.38671875" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="7.3515625" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="7.7265625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="15.9921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="2.15234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.95703125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.9296875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.43359375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.22265625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.1484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.0546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="8.91796875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="27.59765625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="6.49609375" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="14.66796875" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="7.38671875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="9.76953125" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="7.7265625" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="15.9921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -273,13 +280,16 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
         <v>2.0180001E7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -293,21 +303,21 @@
       <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="G2"/>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
+      <c r="H2"/>
       <c r="I2" t="s">
         <v>22</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="n">
         <v>10.0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
       </c>
       <c r="M2" t="s">
         <v>25</v>
@@ -315,47 +325,50 @@
       <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="n">
         <v>5500.0</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>1375.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.0180005E7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.0180006E7</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3" t="s">
         <v>30</v>
       </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3"/>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="n">
+        <v>10.0</v>
       </c>
       <c r="M3" t="s">
         <v>25</v>
@@ -363,110 +376,130 @@
       <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="O3" t="n">
-        <v>51849.0</v>
+      <c r="O3" t="s">
+        <v>34</v>
       </c>
       <c r="P3" t="n">
-        <v>1981.0</v>
+        <v>516189.0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>19811.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.0180006E7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2.0180008E7</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4"/>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="n">
+        <v>16.0</v>
       </c>
       <c r="M4" t="s">
         <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" t="n">
-        <v>516189.0</v>
+        <v>42</v>
+      </c>
+      <c r="O4" t="s">
+        <v>43</v>
       </c>
       <c r="P4" t="n">
-        <v>19811.0</v>
+        <v>524698.0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>55884.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2.0180007E7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2.018001E7</v>
       </c>
       <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="L5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" t="s">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
+      <c r="O5" t="s">
         <v>43</v>
       </c>
-      <c r="G5"/>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" t="n">
-        <v>47552.0</v>
-      </c>
       <c r="P5" t="n">
-        <v>2145.0</v>
+        <v>11651.0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1681.0</v>
       </c>
     </row>
     <row r="6"/>
+    <row r="7">
+      <c r="O7" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1058038.0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>78751.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>